<commit_message>
Updated base rate date format
</commit_message>
<xml_diff>
--- a/rawData/Statista EZB Leitzins Entwicklung.xlsx
+++ b/rawData/Statista EZB Leitzins Entwicklung.xlsx
@@ -362,12 +362,12 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="4"/>
@@ -745,14 +745,14 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
@@ -761,12 +761,12 @@
       <c r="C10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
@@ -775,12 +775,12 @@
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
@@ -789,12 +789,12 @@
       <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
@@ -803,12 +803,12 @@
       <c r="C13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
@@ -817,12 +817,12 @@
       <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
@@ -831,12 +831,12 @@
       <c r="C15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
@@ -845,12 +845,12 @@
       <c r="C16" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
@@ -859,12 +859,12 @@
       <c r="C17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
     </row>
     <row r="18" spans="2:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
@@ -873,39 +873,39 @@
       <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
@@ -914,12 +914,12 @@
       <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
@@ -928,12 +928,12 @@
       <c r="C23" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
@@ -942,12 +942,12 @@
       <c r="C24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
@@ -956,1476 +956,1476 @@
       <c r="C25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
     </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-      <c r="J36" s="13"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
     </row>
     <row r="38" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
     </row>
     <row r="39" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
     </row>
     <row r="40" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
     </row>
     <row r="41" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
     </row>
     <row r="42" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+      <c r="H42" s="15"/>
+      <c r="I42" s="15"/>
+      <c r="J42" s="15"/>
     </row>
     <row r="43" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15"/>
     </row>
     <row r="44" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="15"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="15"/>
+      <c r="J44" s="15"/>
     </row>
     <row r="45" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
+      <c r="E45" s="15"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="15"/>
+      <c r="H45" s="15"/>
+      <c r="I45" s="15"/>
+      <c r="J45" s="15"/>
     </row>
     <row r="46" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="15"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="15"/>
+      <c r="J46" s="15"/>
     </row>
     <row r="47" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="15"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="15"/>
+      <c r="J47" s="15"/>
     </row>
     <row r="48" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15"/>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15"/>
     </row>
     <row r="49" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
+      <c r="E49" s="15"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="15"/>
+      <c r="H49" s="15"/>
+      <c r="I49" s="15"/>
+      <c r="J49" s="15"/>
     </row>
     <row r="50" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
+      <c r="E50" s="15"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="15"/>
+      <c r="H50" s="15"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
     </row>
     <row r="51" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
     </row>
     <row r="52" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
+      <c r="E52" s="15"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="15"/>
+      <c r="H52" s="15"/>
+      <c r="I52" s="15"/>
+      <c r="J52" s="15"/>
     </row>
     <row r="53" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
+      <c r="E53" s="15"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="15"/>
+      <c r="H53" s="15"/>
+      <c r="I53" s="15"/>
+      <c r="J53" s="15"/>
     </row>
     <row r="54" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="15"/>
     </row>
     <row r="55" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="15"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
     </row>
     <row r="56" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
+      <c r="E56" s="15"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="15"/>
+      <c r="H56" s="15"/>
+      <c r="I56" s="15"/>
+      <c r="J56" s="15"/>
     </row>
     <row r="57" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="15"/>
+      <c r="H57" s="15"/>
+      <c r="I57" s="15"/>
+      <c r="J57" s="15"/>
     </row>
     <row r="58" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
+      <c r="E58" s="15"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
     </row>
     <row r="59" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
     </row>
     <row r="60" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="13"/>
+      <c r="E60" s="15"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="15"/>
+      <c r="H60" s="15"/>
+      <c r="I60" s="15"/>
+      <c r="J60" s="15"/>
     </row>
     <row r="61" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="15"/>
+      <c r="H61" s="15"/>
+      <c r="I61" s="15"/>
+      <c r="J61" s="15"/>
     </row>
     <row r="62" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
+      <c r="E62" s="15"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="15"/>
+      <c r="H62" s="15"/>
+      <c r="I62" s="15"/>
+      <c r="J62" s="15"/>
     </row>
     <row r="63" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="15"/>
     </row>
     <row r="64" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
+      <c r="E64" s="15"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="15"/>
+      <c r="H64" s="15"/>
+      <c r="I64" s="15"/>
+      <c r="J64" s="15"/>
     </row>
     <row r="65" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
+      <c r="E65" s="15"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="15"/>
+      <c r="H65" s="15"/>
+      <c r="I65" s="15"/>
+      <c r="J65" s="15"/>
     </row>
     <row r="66" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="13"/>
+      <c r="E66" s="15"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="15"/>
+      <c r="H66" s="15"/>
+      <c r="I66" s="15"/>
+      <c r="J66" s="15"/>
     </row>
     <row r="67" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="15"/>
     </row>
     <row r="68" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
+      <c r="E68" s="15"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="15"/>
+      <c r="H68" s="15"/>
+      <c r="I68" s="15"/>
+      <c r="J68" s="15"/>
     </row>
     <row r="69" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13"/>
-      <c r="H69" s="13"/>
-      <c r="I69" s="13"/>
-      <c r="J69" s="13"/>
+      <c r="E69" s="15"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="15"/>
+      <c r="H69" s="15"/>
+      <c r="I69" s="15"/>
+      <c r="J69" s="15"/>
     </row>
     <row r="70" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13"/>
-      <c r="H70" s="13"/>
-      <c r="I70" s="13"/>
-      <c r="J70" s="13"/>
+      <c r="E70" s="15"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="15"/>
+      <c r="H70" s="15"/>
+      <c r="I70" s="15"/>
+      <c r="J70" s="15"/>
     </row>
     <row r="71" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="13"/>
-      <c r="H71" s="13"/>
-      <c r="I71" s="13"/>
-      <c r="J71" s="13"/>
+      <c r="E71" s="15"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="15"/>
+      <c r="H71" s="15"/>
+      <c r="I71" s="15"/>
+      <c r="J71" s="15"/>
     </row>
     <row r="72" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
-      <c r="H72" s="13"/>
-      <c r="I72" s="13"/>
-      <c r="J72" s="13"/>
+      <c r="E72" s="15"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="15"/>
+      <c r="H72" s="15"/>
+      <c r="I72" s="15"/>
+      <c r="J72" s="15"/>
     </row>
     <row r="73" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
-      <c r="H73" s="13"/>
-      <c r="I73" s="13"/>
-      <c r="J73" s="13"/>
+      <c r="E73" s="15"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="15"/>
+      <c r="H73" s="15"/>
+      <c r="I73" s="15"/>
+      <c r="J73" s="15"/>
     </row>
     <row r="74" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E74" s="13"/>
-      <c r="F74" s="13"/>
-      <c r="G74" s="13"/>
-      <c r="H74" s="13"/>
-      <c r="I74" s="13"/>
-      <c r="J74" s="13"/>
+      <c r="E74" s="15"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="15"/>
+      <c r="H74" s="15"/>
+      <c r="I74" s="15"/>
+      <c r="J74" s="15"/>
     </row>
     <row r="75" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E75" s="13"/>
-      <c r="F75" s="13"/>
-      <c r="G75" s="13"/>
-      <c r="H75" s="13"/>
-      <c r="I75" s="13"/>
-      <c r="J75" s="13"/>
+      <c r="E75" s="15"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="15"/>
+      <c r="H75" s="15"/>
+      <c r="I75" s="15"/>
+      <c r="J75" s="15"/>
     </row>
     <row r="76" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E76" s="13"/>
-      <c r="F76" s="13"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="13"/>
-      <c r="I76" s="13"/>
-      <c r="J76" s="13"/>
+      <c r="E76" s="15"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="15"/>
+      <c r="H76" s="15"/>
+      <c r="I76" s="15"/>
+      <c r="J76" s="15"/>
     </row>
     <row r="77" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E77" s="13"/>
-      <c r="F77" s="13"/>
-      <c r="G77" s="13"/>
-      <c r="H77" s="13"/>
-      <c r="I77" s="13"/>
-      <c r="J77" s="13"/>
+      <c r="E77" s="15"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="15"/>
+      <c r="H77" s="15"/>
+      <c r="I77" s="15"/>
+      <c r="J77" s="15"/>
     </row>
     <row r="78" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E78" s="13"/>
-      <c r="F78" s="13"/>
-      <c r="G78" s="13"/>
-      <c r="H78" s="13"/>
-      <c r="I78" s="13"/>
-      <c r="J78" s="13"/>
+      <c r="E78" s="15"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="15"/>
+      <c r="H78" s="15"/>
+      <c r="I78" s="15"/>
+      <c r="J78" s="15"/>
     </row>
     <row r="79" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E79" s="13"/>
-      <c r="F79" s="13"/>
-      <c r="G79" s="13"/>
-      <c r="H79" s="13"/>
-      <c r="I79" s="13"/>
-      <c r="J79" s="13"/>
+      <c r="E79" s="15"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="15"/>
+      <c r="H79" s="15"/>
+      <c r="I79" s="15"/>
+      <c r="J79" s="15"/>
     </row>
     <row r="80" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E80" s="13"/>
-      <c r="F80" s="13"/>
-      <c r="G80" s="13"/>
-      <c r="H80" s="13"/>
-      <c r="I80" s="13"/>
-      <c r="J80" s="13"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="15"/>
+      <c r="H80" s="15"/>
+      <c r="I80" s="15"/>
+      <c r="J80" s="15"/>
     </row>
     <row r="81" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E81" s="13"/>
-      <c r="F81" s="13"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="13"/>
-      <c r="I81" s="13"/>
-      <c r="J81" s="13"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="15"/>
+      <c r="H81" s="15"/>
+      <c r="I81" s="15"/>
+      <c r="J81" s="15"/>
     </row>
     <row r="82" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E82" s="13"/>
-      <c r="F82" s="13"/>
-      <c r="G82" s="13"/>
-      <c r="H82" s="13"/>
-      <c r="I82" s="13"/>
-      <c r="J82" s="13"/>
+      <c r="E82" s="15"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="15"/>
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15"/>
     </row>
     <row r="83" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E83" s="13"/>
-      <c r="F83" s="13"/>
-      <c r="G83" s="13"/>
-      <c r="H83" s="13"/>
-      <c r="I83" s="13"/>
-      <c r="J83" s="13"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="15"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
     </row>
     <row r="84" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E84" s="13"/>
-      <c r="F84" s="13"/>
-      <c r="G84" s="13"/>
-      <c r="H84" s="13"/>
-      <c r="I84" s="13"/>
-      <c r="J84" s="13"/>
+      <c r="E84" s="15"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="15"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
+      <c r="J84" s="15"/>
     </row>
     <row r="85" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E85" s="13"/>
-      <c r="F85" s="13"/>
-      <c r="G85" s="13"/>
-      <c r="H85" s="13"/>
-      <c r="I85" s="13"/>
-      <c r="J85" s="13"/>
+      <c r="E85" s="15"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="15"/>
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
     </row>
     <row r="86" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E86" s="13"/>
-      <c r="F86" s="13"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="13"/>
-      <c r="I86" s="13"/>
-      <c r="J86" s="13"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
     </row>
     <row r="87" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E87" s="13"/>
-      <c r="F87" s="13"/>
-      <c r="G87" s="13"/>
-      <c r="H87" s="13"/>
-      <c r="I87" s="13"/>
-      <c r="J87" s="13"/>
+      <c r="E87" s="15"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="15"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
+      <c r="J87" s="15"/>
     </row>
     <row r="88" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E88" s="13"/>
-      <c r="F88" s="13"/>
-      <c r="G88" s="13"/>
-      <c r="H88" s="13"/>
-      <c r="I88" s="13"/>
-      <c r="J88" s="13"/>
+      <c r="E88" s="15"/>
+      <c r="F88" s="15"/>
+      <c r="G88" s="15"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
+      <c r="J88" s="15"/>
     </row>
     <row r="89" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E89" s="13"/>
-      <c r="F89" s="13"/>
-      <c r="G89" s="13"/>
-      <c r="H89" s="13"/>
-      <c r="I89" s="13"/>
-      <c r="J89" s="13"/>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="15"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
     </row>
     <row r="90" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E90" s="13"/>
-      <c r="F90" s="13"/>
-      <c r="G90" s="13"/>
-      <c r="H90" s="13"/>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
+      <c r="E90" s="15"/>
+      <c r="F90" s="15"/>
+      <c r="G90" s="15"/>
+      <c r="H90" s="15"/>
+      <c r="I90" s="15"/>
+      <c r="J90" s="15"/>
     </row>
     <row r="91" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E91" s="13"/>
-      <c r="F91" s="13"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="13"/>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
+      <c r="E91" s="15"/>
+      <c r="F91" s="15"/>
+      <c r="G91" s="15"/>
+      <c r="H91" s="15"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
     </row>
     <row r="92" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E92" s="13"/>
-      <c r="F92" s="13"/>
-      <c r="G92" s="13"/>
-      <c r="H92" s="13"/>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
+      <c r="E92" s="15"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="15"/>
+      <c r="H92" s="15"/>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
     </row>
     <row r="93" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E93" s="13"/>
-      <c r="F93" s="13"/>
-      <c r="G93" s="13"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
+      <c r="E93" s="15"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="15"/>
+      <c r="H93" s="15"/>
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
     </row>
     <row r="94" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E94" s="13"/>
-      <c r="F94" s="13"/>
-      <c r="G94" s="13"/>
-      <c r="H94" s="13"/>
-      <c r="I94" s="13"/>
-      <c r="J94" s="13"/>
+      <c r="E94" s="15"/>
+      <c r="F94" s="15"/>
+      <c r="G94" s="15"/>
+      <c r="H94" s="15"/>
+      <c r="I94" s="15"/>
+      <c r="J94" s="15"/>
     </row>
     <row r="95" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E95" s="13"/>
-      <c r="F95" s="13"/>
-      <c r="G95" s="13"/>
-      <c r="H95" s="13"/>
-      <c r="I95" s="13"/>
-      <c r="J95" s="13"/>
+      <c r="E95" s="15"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="15"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+      <c r="J95" s="15"/>
     </row>
     <row r="96" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E96" s="13"/>
-      <c r="F96" s="13"/>
-      <c r="G96" s="13"/>
-      <c r="H96" s="13"/>
-      <c r="I96" s="13"/>
-      <c r="J96" s="13"/>
+      <c r="E96" s="15"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="15"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15"/>
+      <c r="J96" s="15"/>
     </row>
     <row r="97" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E97" s="13"/>
-      <c r="F97" s="13"/>
-      <c r="G97" s="13"/>
-      <c r="H97" s="13"/>
-      <c r="I97" s="13"/>
-      <c r="J97" s="13"/>
+      <c r="E97" s="15"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="15"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="15"/>
+      <c r="J97" s="15"/>
     </row>
     <row r="98" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E98" s="13"/>
-      <c r="F98" s="13"/>
-      <c r="G98" s="13"/>
-      <c r="H98" s="13"/>
-      <c r="I98" s="13"/>
-      <c r="J98" s="13"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="15"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="15"/>
     </row>
     <row r="99" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E99" s="13"/>
-      <c r="F99" s="13"/>
-      <c r="G99" s="13"/>
-      <c r="H99" s="13"/>
-      <c r="I99" s="13"/>
-      <c r="J99" s="13"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="15"/>
+      <c r="H99" s="15"/>
+      <c r="I99" s="15"/>
+      <c r="J99" s="15"/>
     </row>
     <row r="100" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E100" s="13"/>
-      <c r="F100" s="13"/>
-      <c r="G100" s="13"/>
-      <c r="H100" s="13"/>
-      <c r="I100" s="13"/>
-      <c r="J100" s="13"/>
+      <c r="E100" s="15"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="15"/>
+      <c r="I100" s="15"/>
+      <c r="J100" s="15"/>
     </row>
     <row r="101" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E101" s="13"/>
-      <c r="F101" s="13"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="13"/>
-      <c r="I101" s="13"/>
-      <c r="J101" s="13"/>
+      <c r="E101" s="15"/>
+      <c r="F101" s="15"/>
+      <c r="G101" s="15"/>
+      <c r="H101" s="15"/>
+      <c r="I101" s="15"/>
+      <c r="J101" s="15"/>
     </row>
     <row r="102" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E102" s="13"/>
-      <c r="F102" s="13"/>
-      <c r="G102" s="13"/>
-      <c r="H102" s="13"/>
-      <c r="I102" s="13"/>
-      <c r="J102" s="13"/>
+      <c r="E102" s="15"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="15"/>
+      <c r="I102" s="15"/>
+      <c r="J102" s="15"/>
     </row>
     <row r="103" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E103" s="13"/>
-      <c r="F103" s="13"/>
-      <c r="G103" s="13"/>
-      <c r="H103" s="13"/>
-      <c r="I103" s="13"/>
-      <c r="J103" s="13"/>
+      <c r="E103" s="15"/>
+      <c r="F103" s="15"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="15"/>
+      <c r="I103" s="15"/>
+      <c r="J103" s="15"/>
     </row>
     <row r="104" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E104" s="13"/>
-      <c r="F104" s="13"/>
-      <c r="G104" s="13"/>
-      <c r="H104" s="13"/>
-      <c r="I104" s="13"/>
-      <c r="J104" s="13"/>
+      <c r="E104" s="15"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="15"/>
+      <c r="H104" s="15"/>
+      <c r="I104" s="15"/>
+      <c r="J104" s="15"/>
     </row>
     <row r="105" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E105" s="13"/>
-      <c r="F105" s="13"/>
-      <c r="G105" s="13"/>
-      <c r="H105" s="13"/>
-      <c r="I105" s="13"/>
-      <c r="J105" s="13"/>
+      <c r="E105" s="15"/>
+      <c r="F105" s="15"/>
+      <c r="G105" s="15"/>
+      <c r="H105" s="15"/>
+      <c r="I105" s="15"/>
+      <c r="J105" s="15"/>
     </row>
     <row r="106" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E106" s="13"/>
-      <c r="F106" s="13"/>
-      <c r="G106" s="13"/>
-      <c r="H106" s="13"/>
-      <c r="I106" s="13"/>
-      <c r="J106" s="13"/>
+      <c r="E106" s="15"/>
+      <c r="F106" s="15"/>
+      <c r="G106" s="15"/>
+      <c r="H106" s="15"/>
+      <c r="I106" s="15"/>
+      <c r="J106" s="15"/>
     </row>
     <row r="107" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E107" s="13"/>
-      <c r="F107" s="13"/>
-      <c r="G107" s="13"/>
-      <c r="H107" s="13"/>
-      <c r="I107" s="13"/>
-      <c r="J107" s="13"/>
+      <c r="E107" s="15"/>
+      <c r="F107" s="15"/>
+      <c r="G107" s="15"/>
+      <c r="H107" s="15"/>
+      <c r="I107" s="15"/>
+      <c r="J107" s="15"/>
     </row>
     <row r="108" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E108" s="13"/>
-      <c r="F108" s="13"/>
-      <c r="G108" s="13"/>
-      <c r="H108" s="13"/>
-      <c r="I108" s="13"/>
-      <c r="J108" s="13"/>
+      <c r="E108" s="15"/>
+      <c r="F108" s="15"/>
+      <c r="G108" s="15"/>
+      <c r="H108" s="15"/>
+      <c r="I108" s="15"/>
+      <c r="J108" s="15"/>
     </row>
     <row r="109" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E109" s="13"/>
-      <c r="F109" s="13"/>
-      <c r="G109" s="13"/>
-      <c r="H109" s="13"/>
-      <c r="I109" s="13"/>
-      <c r="J109" s="13"/>
+      <c r="E109" s="15"/>
+      <c r="F109" s="15"/>
+      <c r="G109" s="15"/>
+      <c r="H109" s="15"/>
+      <c r="I109" s="15"/>
+      <c r="J109" s="15"/>
     </row>
     <row r="110" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E110" s="13"/>
-      <c r="F110" s="13"/>
-      <c r="G110" s="13"/>
-      <c r="H110" s="13"/>
-      <c r="I110" s="13"/>
-      <c r="J110" s="13"/>
+      <c r="E110" s="15"/>
+      <c r="F110" s="15"/>
+      <c r="G110" s="15"/>
+      <c r="H110" s="15"/>
+      <c r="I110" s="15"/>
+      <c r="J110" s="15"/>
     </row>
     <row r="111" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E111" s="13"/>
-      <c r="F111" s="13"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="13"/>
-      <c r="I111" s="13"/>
-      <c r="J111" s="13"/>
+      <c r="E111" s="15"/>
+      <c r="F111" s="15"/>
+      <c r="G111" s="15"/>
+      <c r="H111" s="15"/>
+      <c r="I111" s="15"/>
+      <c r="J111" s="15"/>
     </row>
     <row r="112" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E112" s="13"/>
-      <c r="F112" s="13"/>
-      <c r="G112" s="13"/>
-      <c r="H112" s="13"/>
-      <c r="I112" s="13"/>
-      <c r="J112" s="13"/>
+      <c r="E112" s="15"/>
+      <c r="F112" s="15"/>
+      <c r="G112" s="15"/>
+      <c r="H112" s="15"/>
+      <c r="I112" s="15"/>
+      <c r="J112" s="15"/>
     </row>
     <row r="113" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E113" s="13"/>
-      <c r="F113" s="13"/>
-      <c r="G113" s="13"/>
-      <c r="H113" s="13"/>
-      <c r="I113" s="13"/>
-      <c r="J113" s="13"/>
+      <c r="E113" s="15"/>
+      <c r="F113" s="15"/>
+      <c r="G113" s="15"/>
+      <c r="H113" s="15"/>
+      <c r="I113" s="15"/>
+      <c r="J113" s="15"/>
     </row>
     <row r="114" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E114" s="13"/>
-      <c r="F114" s="13"/>
-      <c r="G114" s="13"/>
-      <c r="H114" s="13"/>
-      <c r="I114" s="13"/>
-      <c r="J114" s="13"/>
+      <c r="E114" s="15"/>
+      <c r="F114" s="15"/>
+      <c r="G114" s="15"/>
+      <c r="H114" s="15"/>
+      <c r="I114" s="15"/>
+      <c r="J114" s="15"/>
     </row>
     <row r="115" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E115" s="13"/>
-      <c r="F115" s="13"/>
-      <c r="G115" s="13"/>
-      <c r="H115" s="13"/>
-      <c r="I115" s="13"/>
-      <c r="J115" s="13"/>
+      <c r="E115" s="15"/>
+      <c r="F115" s="15"/>
+      <c r="G115" s="15"/>
+      <c r="H115" s="15"/>
+      <c r="I115" s="15"/>
+      <c r="J115" s="15"/>
     </row>
     <row r="116" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E116" s="13"/>
-      <c r="F116" s="13"/>
-      <c r="G116" s="13"/>
-      <c r="H116" s="13"/>
-      <c r="I116" s="13"/>
-      <c r="J116" s="13"/>
+      <c r="E116" s="15"/>
+      <c r="F116" s="15"/>
+      <c r="G116" s="15"/>
+      <c r="H116" s="15"/>
+      <c r="I116" s="15"/>
+      <c r="J116" s="15"/>
     </row>
     <row r="117" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E117" s="13"/>
-      <c r="F117" s="13"/>
-      <c r="G117" s="13"/>
-      <c r="H117" s="13"/>
-      <c r="I117" s="13"/>
-      <c r="J117" s="13"/>
+      <c r="E117" s="15"/>
+      <c r="F117" s="15"/>
+      <c r="G117" s="15"/>
+      <c r="H117" s="15"/>
+      <c r="I117" s="15"/>
+      <c r="J117" s="15"/>
     </row>
     <row r="118" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E118" s="13"/>
-      <c r="F118" s="13"/>
-      <c r="G118" s="13"/>
-      <c r="H118" s="13"/>
-      <c r="I118" s="13"/>
-      <c r="J118" s="13"/>
+      <c r="E118" s="15"/>
+      <c r="F118" s="15"/>
+      <c r="G118" s="15"/>
+      <c r="H118" s="15"/>
+      <c r="I118" s="15"/>
+      <c r="J118" s="15"/>
     </row>
     <row r="119" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E119" s="13"/>
-      <c r="F119" s="13"/>
-      <c r="G119" s="13"/>
-      <c r="H119" s="13"/>
-      <c r="I119" s="13"/>
-      <c r="J119" s="13"/>
+      <c r="E119" s="15"/>
+      <c r="F119" s="15"/>
+      <c r="G119" s="15"/>
+      <c r="H119" s="15"/>
+      <c r="I119" s="15"/>
+      <c r="J119" s="15"/>
     </row>
     <row r="120" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E120" s="13"/>
-      <c r="F120" s="13"/>
-      <c r="G120" s="13"/>
-      <c r="H120" s="13"/>
-      <c r="I120" s="13"/>
-      <c r="J120" s="13"/>
+      <c r="E120" s="15"/>
+      <c r="F120" s="15"/>
+      <c r="G120" s="15"/>
+      <c r="H120" s="15"/>
+      <c r="I120" s="15"/>
+      <c r="J120" s="15"/>
     </row>
     <row r="121" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E121" s="13"/>
-      <c r="F121" s="13"/>
-      <c r="G121" s="13"/>
-      <c r="H121" s="13"/>
-      <c r="I121" s="13"/>
-      <c r="J121" s="13"/>
+      <c r="E121" s="15"/>
+      <c r="F121" s="15"/>
+      <c r="G121" s="15"/>
+      <c r="H121" s="15"/>
+      <c r="I121" s="15"/>
+      <c r="J121" s="15"/>
     </row>
     <row r="122" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E122" s="13"/>
-      <c r="F122" s="13"/>
-      <c r="G122" s="13"/>
-      <c r="H122" s="13"/>
-      <c r="I122" s="13"/>
-      <c r="J122" s="13"/>
+      <c r="E122" s="15"/>
+      <c r="F122" s="15"/>
+      <c r="G122" s="15"/>
+      <c r="H122" s="15"/>
+      <c r="I122" s="15"/>
+      <c r="J122" s="15"/>
     </row>
     <row r="123" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E123" s="13"/>
-      <c r="F123" s="13"/>
-      <c r="G123" s="13"/>
-      <c r="H123" s="13"/>
-      <c r="I123" s="13"/>
-      <c r="J123" s="13"/>
+      <c r="E123" s="15"/>
+      <c r="F123" s="15"/>
+      <c r="G123" s="15"/>
+      <c r="H123" s="15"/>
+      <c r="I123" s="15"/>
+      <c r="J123" s="15"/>
     </row>
     <row r="124" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E124" s="13"/>
-      <c r="F124" s="13"/>
-      <c r="G124" s="13"/>
-      <c r="H124" s="13"/>
-      <c r="I124" s="13"/>
-      <c r="J124" s="13"/>
+      <c r="E124" s="15"/>
+      <c r="F124" s="15"/>
+      <c r="G124" s="15"/>
+      <c r="H124" s="15"/>
+      <c r="I124" s="15"/>
+      <c r="J124" s="15"/>
     </row>
     <row r="125" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E125" s="13"/>
-      <c r="F125" s="13"/>
-      <c r="G125" s="13"/>
-      <c r="H125" s="13"/>
-      <c r="I125" s="13"/>
-      <c r="J125" s="13"/>
+      <c r="E125" s="15"/>
+      <c r="F125" s="15"/>
+      <c r="G125" s="15"/>
+      <c r="H125" s="15"/>
+      <c r="I125" s="15"/>
+      <c r="J125" s="15"/>
     </row>
     <row r="126" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E126" s="13"/>
-      <c r="F126" s="13"/>
-      <c r="G126" s="13"/>
-      <c r="H126" s="13"/>
-      <c r="I126" s="13"/>
-      <c r="J126" s="13"/>
+      <c r="E126" s="15"/>
+      <c r="F126" s="15"/>
+      <c r="G126" s="15"/>
+      <c r="H126" s="15"/>
+      <c r="I126" s="15"/>
+      <c r="J126" s="15"/>
     </row>
     <row r="127" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E127" s="13"/>
-      <c r="F127" s="13"/>
-      <c r="G127" s="13"/>
-      <c r="H127" s="13"/>
-      <c r="I127" s="13"/>
-      <c r="J127" s="13"/>
+      <c r="E127" s="15"/>
+      <c r="F127" s="15"/>
+      <c r="G127" s="15"/>
+      <c r="H127" s="15"/>
+      <c r="I127" s="15"/>
+      <c r="J127" s="15"/>
     </row>
     <row r="128" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E128" s="13"/>
-      <c r="F128" s="13"/>
-      <c r="G128" s="13"/>
-      <c r="H128" s="13"/>
-      <c r="I128" s="13"/>
-      <c r="J128" s="13"/>
+      <c r="E128" s="15"/>
+      <c r="F128" s="15"/>
+      <c r="G128" s="15"/>
+      <c r="H128" s="15"/>
+      <c r="I128" s="15"/>
+      <c r="J128" s="15"/>
     </row>
     <row r="129" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E129" s="13"/>
-      <c r="F129" s="13"/>
-      <c r="G129" s="13"/>
-      <c r="H129" s="13"/>
-      <c r="I129" s="13"/>
-      <c r="J129" s="13"/>
+      <c r="E129" s="15"/>
+      <c r="F129" s="15"/>
+      <c r="G129" s="15"/>
+      <c r="H129" s="15"/>
+      <c r="I129" s="15"/>
+      <c r="J129" s="15"/>
     </row>
     <row r="130" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E130" s="13"/>
-      <c r="F130" s="13"/>
-      <c r="G130" s="13"/>
-      <c r="H130" s="13"/>
-      <c r="I130" s="13"/>
-      <c r="J130" s="13"/>
+      <c r="E130" s="15"/>
+      <c r="F130" s="15"/>
+      <c r="G130" s="15"/>
+      <c r="H130" s="15"/>
+      <c r="I130" s="15"/>
+      <c r="J130" s="15"/>
     </row>
     <row r="131" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E131" s="13"/>
-      <c r="F131" s="13"/>
-      <c r="G131" s="13"/>
-      <c r="H131" s="13"/>
-      <c r="I131" s="13"/>
-      <c r="J131" s="13"/>
+      <c r="E131" s="15"/>
+      <c r="F131" s="15"/>
+      <c r="G131" s="15"/>
+      <c r="H131" s="15"/>
+      <c r="I131" s="15"/>
+      <c r="J131" s="15"/>
     </row>
     <row r="132" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E132" s="13"/>
-      <c r="F132" s="13"/>
-      <c r="G132" s="13"/>
-      <c r="H132" s="13"/>
-      <c r="I132" s="13"/>
-      <c r="J132" s="13"/>
+      <c r="E132" s="15"/>
+      <c r="F132" s="15"/>
+      <c r="G132" s="15"/>
+      <c r="H132" s="15"/>
+      <c r="I132" s="15"/>
+      <c r="J132" s="15"/>
     </row>
     <row r="133" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E133" s="13"/>
-      <c r="F133" s="13"/>
-      <c r="G133" s="13"/>
-      <c r="H133" s="13"/>
-      <c r="I133" s="13"/>
-      <c r="J133" s="13"/>
+      <c r="E133" s="15"/>
+      <c r="F133" s="15"/>
+      <c r="G133" s="15"/>
+      <c r="H133" s="15"/>
+      <c r="I133" s="15"/>
+      <c r="J133" s="15"/>
     </row>
     <row r="134" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E134" s="13"/>
-      <c r="F134" s="13"/>
-      <c r="G134" s="13"/>
-      <c r="H134" s="13"/>
-      <c r="I134" s="13"/>
-      <c r="J134" s="13"/>
+      <c r="E134" s="15"/>
+      <c r="F134" s="15"/>
+      <c r="G134" s="15"/>
+      <c r="H134" s="15"/>
+      <c r="I134" s="15"/>
+      <c r="J134" s="15"/>
     </row>
     <row r="135" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E135" s="13"/>
-      <c r="F135" s="13"/>
-      <c r="G135" s="13"/>
-      <c r="H135" s="13"/>
-      <c r="I135" s="13"/>
-      <c r="J135" s="13"/>
+      <c r="E135" s="15"/>
+      <c r="F135" s="15"/>
+      <c r="G135" s="15"/>
+      <c r="H135" s="15"/>
+      <c r="I135" s="15"/>
+      <c r="J135" s="15"/>
     </row>
     <row r="136" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E136" s="13"/>
-      <c r="F136" s="13"/>
-      <c r="G136" s="13"/>
-      <c r="H136" s="13"/>
-      <c r="I136" s="13"/>
-      <c r="J136" s="13"/>
+      <c r="E136" s="15"/>
+      <c r="F136" s="15"/>
+      <c r="G136" s="15"/>
+      <c r="H136" s="15"/>
+      <c r="I136" s="15"/>
+      <c r="J136" s="15"/>
     </row>
     <row r="137" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E137" s="13"/>
-      <c r="F137" s="13"/>
-      <c r="G137" s="13"/>
-      <c r="H137" s="13"/>
-      <c r="I137" s="13"/>
-      <c r="J137" s="13"/>
+      <c r="E137" s="15"/>
+      <c r="F137" s="15"/>
+      <c r="G137" s="15"/>
+      <c r="H137" s="15"/>
+      <c r="I137" s="15"/>
+      <c r="J137" s="15"/>
     </row>
     <row r="138" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E138" s="13"/>
-      <c r="F138" s="13"/>
-      <c r="G138" s="13"/>
-      <c r="H138" s="13"/>
-      <c r="I138" s="13"/>
-      <c r="J138" s="13"/>
+      <c r="E138" s="15"/>
+      <c r="F138" s="15"/>
+      <c r="G138" s="15"/>
+      <c r="H138" s="15"/>
+      <c r="I138" s="15"/>
+      <c r="J138" s="15"/>
     </row>
     <row r="139" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E139" s="13"/>
-      <c r="F139" s="13"/>
-      <c r="G139" s="13"/>
-      <c r="H139" s="13"/>
-      <c r="I139" s="13"/>
-      <c r="J139" s="13"/>
+      <c r="E139" s="15"/>
+      <c r="F139" s="15"/>
+      <c r="G139" s="15"/>
+      <c r="H139" s="15"/>
+      <c r="I139" s="15"/>
+      <c r="J139" s="15"/>
     </row>
     <row r="140" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E140" s="13"/>
-      <c r="F140" s="13"/>
-      <c r="G140" s="13"/>
-      <c r="H140" s="13"/>
-      <c r="I140" s="13"/>
-      <c r="J140" s="13"/>
+      <c r="E140" s="15"/>
+      <c r="F140" s="15"/>
+      <c r="G140" s="15"/>
+      <c r="H140" s="15"/>
+      <c r="I140" s="15"/>
+      <c r="J140" s="15"/>
     </row>
     <row r="141" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E141" s="13"/>
-      <c r="F141" s="13"/>
-      <c r="G141" s="13"/>
-      <c r="H141" s="13"/>
-      <c r="I141" s="13"/>
-      <c r="J141" s="13"/>
+      <c r="E141" s="15"/>
+      <c r="F141" s="15"/>
+      <c r="G141" s="15"/>
+      <c r="H141" s="15"/>
+      <c r="I141" s="15"/>
+      <c r="J141" s="15"/>
     </row>
     <row r="142" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E142" s="13"/>
-      <c r="F142" s="13"/>
-      <c r="G142" s="13"/>
-      <c r="H142" s="13"/>
-      <c r="I142" s="13"/>
-      <c r="J142" s="13"/>
+      <c r="E142" s="15"/>
+      <c r="F142" s="15"/>
+      <c r="G142" s="15"/>
+      <c r="H142" s="15"/>
+      <c r="I142" s="15"/>
+      <c r="J142" s="15"/>
     </row>
     <row r="143" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E143" s="13"/>
-      <c r="F143" s="13"/>
-      <c r="G143" s="13"/>
-      <c r="H143" s="13"/>
-      <c r="I143" s="13"/>
-      <c r="J143" s="13"/>
+      <c r="E143" s="15"/>
+      <c r="F143" s="15"/>
+      <c r="G143" s="15"/>
+      <c r="H143" s="15"/>
+      <c r="I143" s="15"/>
+      <c r="J143" s="15"/>
     </row>
     <row r="144" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E144" s="13"/>
-      <c r="F144" s="13"/>
-      <c r="G144" s="13"/>
-      <c r="H144" s="13"/>
-      <c r="I144" s="13"/>
-      <c r="J144" s="13"/>
+      <c r="E144" s="15"/>
+      <c r="F144" s="15"/>
+      <c r="G144" s="15"/>
+      <c r="H144" s="15"/>
+      <c r="I144" s="15"/>
+      <c r="J144" s="15"/>
     </row>
     <row r="145" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E145" s="13"/>
-      <c r="F145" s="13"/>
-      <c r="G145" s="13"/>
-      <c r="H145" s="13"/>
-      <c r="I145" s="13"/>
-      <c r="J145" s="13"/>
+      <c r="E145" s="15"/>
+      <c r="F145" s="15"/>
+      <c r="G145" s="15"/>
+      <c r="H145" s="15"/>
+      <c r="I145" s="15"/>
+      <c r="J145" s="15"/>
     </row>
     <row r="146" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E146" s="13"/>
-      <c r="F146" s="13"/>
-      <c r="G146" s="13"/>
-      <c r="H146" s="13"/>
-      <c r="I146" s="13"/>
-      <c r="J146" s="13"/>
+      <c r="E146" s="15"/>
+      <c r="F146" s="15"/>
+      <c r="G146" s="15"/>
+      <c r="H146" s="15"/>
+      <c r="I146" s="15"/>
+      <c r="J146" s="15"/>
     </row>
     <row r="147" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E147" s="13"/>
-      <c r="F147" s="13"/>
-      <c r="G147" s="13"/>
-      <c r="H147" s="13"/>
-      <c r="I147" s="13"/>
-      <c r="J147" s="13"/>
+      <c r="E147" s="15"/>
+      <c r="F147" s="15"/>
+      <c r="G147" s="15"/>
+      <c r="H147" s="15"/>
+      <c r="I147" s="15"/>
+      <c r="J147" s="15"/>
     </row>
     <row r="148" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E148" s="13"/>
-      <c r="F148" s="13"/>
-      <c r="G148" s="13"/>
-      <c r="H148" s="13"/>
-      <c r="I148" s="13"/>
-      <c r="J148" s="13"/>
+      <c r="E148" s="15"/>
+      <c r="F148" s="15"/>
+      <c r="G148" s="15"/>
+      <c r="H148" s="15"/>
+      <c r="I148" s="15"/>
+      <c r="J148" s="15"/>
     </row>
     <row r="149" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E149" s="13"/>
-      <c r="F149" s="13"/>
-      <c r="G149" s="13"/>
-      <c r="H149" s="13"/>
-      <c r="I149" s="13"/>
-      <c r="J149" s="13"/>
+      <c r="E149" s="15"/>
+      <c r="F149" s="15"/>
+      <c r="G149" s="15"/>
+      <c r="H149" s="15"/>
+      <c r="I149" s="15"/>
+      <c r="J149" s="15"/>
     </row>
     <row r="150" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E150" s="13"/>
-      <c r="F150" s="13"/>
-      <c r="G150" s="13"/>
-      <c r="H150" s="13"/>
-      <c r="I150" s="13"/>
-      <c r="J150" s="13"/>
+      <c r="E150" s="15"/>
+      <c r="F150" s="15"/>
+      <c r="G150" s="15"/>
+      <c r="H150" s="15"/>
+      <c r="I150" s="15"/>
+      <c r="J150" s="15"/>
     </row>
     <row r="151" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E151" s="13"/>
-      <c r="F151" s="13"/>
-      <c r="G151" s="13"/>
-      <c r="H151" s="13"/>
-      <c r="I151" s="13"/>
-      <c r="J151" s="13"/>
+      <c r="E151" s="15"/>
+      <c r="F151" s="15"/>
+      <c r="G151" s="15"/>
+      <c r="H151" s="15"/>
+      <c r="I151" s="15"/>
+      <c r="J151" s="15"/>
     </row>
     <row r="152" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E152" s="13"/>
-      <c r="F152" s="13"/>
-      <c r="G152" s="13"/>
-      <c r="H152" s="13"/>
-      <c r="I152" s="13"/>
-      <c r="J152" s="13"/>
+      <c r="E152" s="15"/>
+      <c r="F152" s="15"/>
+      <c r="G152" s="15"/>
+      <c r="H152" s="15"/>
+      <c r="I152" s="15"/>
+      <c r="J152" s="15"/>
     </row>
     <row r="153" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E153" s="13"/>
-      <c r="F153" s="13"/>
-      <c r="G153" s="13"/>
-      <c r="H153" s="13"/>
-      <c r="I153" s="13"/>
-      <c r="J153" s="13"/>
+      <c r="E153" s="15"/>
+      <c r="F153" s="15"/>
+      <c r="G153" s="15"/>
+      <c r="H153" s="15"/>
+      <c r="I153" s="15"/>
+      <c r="J153" s="15"/>
     </row>
     <row r="154" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E154" s="13"/>
-      <c r="F154" s="13"/>
-      <c r="G154" s="13"/>
-      <c r="H154" s="13"/>
-      <c r="I154" s="13"/>
-      <c r="J154" s="13"/>
+      <c r="E154" s="15"/>
+      <c r="F154" s="15"/>
+      <c r="G154" s="15"/>
+      <c r="H154" s="15"/>
+      <c r="I154" s="15"/>
+      <c r="J154" s="15"/>
     </row>
     <row r="155" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E155" s="13"/>
-      <c r="F155" s="13"/>
-      <c r="G155" s="13"/>
-      <c r="H155" s="13"/>
-      <c r="I155" s="13"/>
-      <c r="J155" s="13"/>
+      <c r="E155" s="15"/>
+      <c r="F155" s="15"/>
+      <c r="G155" s="15"/>
+      <c r="H155" s="15"/>
+      <c r="I155" s="15"/>
+      <c r="J155" s="15"/>
     </row>
     <row r="156" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E156" s="13"/>
-      <c r="F156" s="13"/>
-      <c r="G156" s="13"/>
-      <c r="H156" s="13"/>
-      <c r="I156" s="13"/>
-      <c r="J156" s="13"/>
+      <c r="E156" s="15"/>
+      <c r="F156" s="15"/>
+      <c r="G156" s="15"/>
+      <c r="H156" s="15"/>
+      <c r="I156" s="15"/>
+      <c r="J156" s="15"/>
     </row>
     <row r="157" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E157" s="13"/>
-      <c r="F157" s="13"/>
-      <c r="G157" s="13"/>
-      <c r="H157" s="13"/>
-      <c r="I157" s="13"/>
-      <c r="J157" s="13"/>
+      <c r="E157" s="15"/>
+      <c r="F157" s="15"/>
+      <c r="G157" s="15"/>
+      <c r="H157" s="15"/>
+      <c r="I157" s="15"/>
+      <c r="J157" s="15"/>
     </row>
     <row r="158" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E158" s="13"/>
-      <c r="F158" s="13"/>
-      <c r="G158" s="13"/>
-      <c r="H158" s="13"/>
-      <c r="I158" s="13"/>
-      <c r="J158" s="13"/>
+      <c r="E158" s="15"/>
+      <c r="F158" s="15"/>
+      <c r="G158" s="15"/>
+      <c r="H158" s="15"/>
+      <c r="I158" s="15"/>
+      <c r="J158" s="15"/>
     </row>
     <row r="159" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E159" s="13"/>
-      <c r="F159" s="13"/>
-      <c r="G159" s="13"/>
-      <c r="H159" s="13"/>
-      <c r="I159" s="13"/>
-      <c r="J159" s="13"/>
+      <c r="E159" s="15"/>
+      <c r="F159" s="15"/>
+      <c r="G159" s="15"/>
+      <c r="H159" s="15"/>
+      <c r="I159" s="15"/>
+      <c r="J159" s="15"/>
     </row>
     <row r="160" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E160" s="13"/>
-      <c r="F160" s="13"/>
-      <c r="G160" s="13"/>
-      <c r="H160" s="13"/>
-      <c r="I160" s="13"/>
-      <c r="J160" s="13"/>
+      <c r="E160" s="15"/>
+      <c r="F160" s="15"/>
+      <c r="G160" s="15"/>
+      <c r="H160" s="15"/>
+      <c r="I160" s="15"/>
+      <c r="J160" s="15"/>
     </row>
     <row r="161" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E161" s="13"/>
-      <c r="F161" s="13"/>
-      <c r="G161" s="13"/>
-      <c r="H161" s="13"/>
-      <c r="I161" s="13"/>
-      <c r="J161" s="13"/>
+      <c r="E161" s="15"/>
+      <c r="F161" s="15"/>
+      <c r="G161" s="15"/>
+      <c r="H161" s="15"/>
+      <c r="I161" s="15"/>
+      <c r="J161" s="15"/>
     </row>
     <row r="162" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E162" s="13"/>
-      <c r="F162" s="13"/>
-      <c r="G162" s="13"/>
-      <c r="H162" s="13"/>
-      <c r="I162" s="13"/>
-      <c r="J162" s="13"/>
+      <c r="E162" s="15"/>
+      <c r="F162" s="15"/>
+      <c r="G162" s="15"/>
+      <c r="H162" s="15"/>
+      <c r="I162" s="15"/>
+      <c r="J162" s="15"/>
     </row>
     <row r="163" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E163" s="13"/>
-      <c r="F163" s="13"/>
-      <c r="G163" s="13"/>
-      <c r="H163" s="13"/>
-      <c r="I163" s="13"/>
-      <c r="J163" s="13"/>
+      <c r="E163" s="15"/>
+      <c r="F163" s="15"/>
+      <c r="G163" s="15"/>
+      <c r="H163" s="15"/>
+      <c r="I163" s="15"/>
+      <c r="J163" s="15"/>
     </row>
     <row r="164" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E164" s="13"/>
-      <c r="F164" s="13"/>
-      <c r="G164" s="13"/>
-      <c r="H164" s="13"/>
-      <c r="I164" s="13"/>
-      <c r="J164" s="13"/>
+      <c r="E164" s="15"/>
+      <c r="F164" s="15"/>
+      <c r="G164" s="15"/>
+      <c r="H164" s="15"/>
+      <c r="I164" s="15"/>
+      <c r="J164" s="15"/>
     </row>
     <row r="165" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E165" s="13"/>
-      <c r="F165" s="13"/>
-      <c r="G165" s="13"/>
-      <c r="H165" s="13"/>
-      <c r="I165" s="13"/>
-      <c r="J165" s="13"/>
+      <c r="E165" s="15"/>
+      <c r="F165" s="15"/>
+      <c r="G165" s="15"/>
+      <c r="H165" s="15"/>
+      <c r="I165" s="15"/>
+      <c r="J165" s="15"/>
     </row>
     <row r="166" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E166" s="13"/>
-      <c r="F166" s="13"/>
-      <c r="G166" s="13"/>
-      <c r="H166" s="13"/>
-      <c r="I166" s="13"/>
-      <c r="J166" s="13"/>
+      <c r="E166" s="15"/>
+      <c r="F166" s="15"/>
+      <c r="G166" s="15"/>
+      <c r="H166" s="15"/>
+      <c r="I166" s="15"/>
+      <c r="J166" s="15"/>
     </row>
     <row r="167" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E167" s="13"/>
-      <c r="F167" s="13"/>
-      <c r="G167" s="13"/>
-      <c r="H167" s="13"/>
-      <c r="I167" s="13"/>
-      <c r="J167" s="13"/>
+      <c r="E167" s="15"/>
+      <c r="F167" s="15"/>
+      <c r="G167" s="15"/>
+      <c r="H167" s="15"/>
+      <c r="I167" s="15"/>
+      <c r="J167" s="15"/>
     </row>
     <row r="168" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E168" s="13"/>
-      <c r="F168" s="13"/>
-      <c r="G168" s="13"/>
-      <c r="H168" s="13"/>
-      <c r="I168" s="13"/>
-      <c r="J168" s="13"/>
+      <c r="E168" s="15"/>
+      <c r="F168" s="15"/>
+      <c r="G168" s="15"/>
+      <c r="H168" s="15"/>
+      <c r="I168" s="15"/>
+      <c r="J168" s="15"/>
     </row>
     <row r="169" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E169" s="13"/>
-      <c r="F169" s="13"/>
-      <c r="G169" s="13"/>
-      <c r="H169" s="13"/>
-      <c r="I169" s="13"/>
-      <c r="J169" s="13"/>
+      <c r="E169" s="15"/>
+      <c r="F169" s="15"/>
+      <c r="G169" s="15"/>
+      <c r="H169" s="15"/>
+      <c r="I169" s="15"/>
+      <c r="J169" s="15"/>
     </row>
     <row r="170" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E170" s="13"/>
-      <c r="F170" s="13"/>
-      <c r="G170" s="13"/>
-      <c r="H170" s="13"/>
-      <c r="I170" s="13"/>
-      <c r="J170" s="13"/>
+      <c r="E170" s="15"/>
+      <c r="F170" s="15"/>
+      <c r="G170" s="15"/>
+      <c r="H170" s="15"/>
+      <c r="I170" s="15"/>
+      <c r="J170" s="15"/>
     </row>
     <row r="171" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E171" s="13"/>
-      <c r="F171" s="13"/>
-      <c r="G171" s="13"/>
-      <c r="H171" s="13"/>
-      <c r="I171" s="13"/>
-      <c r="J171" s="13"/>
+      <c r="E171" s="15"/>
+      <c r="F171" s="15"/>
+      <c r="G171" s="15"/>
+      <c r="H171" s="15"/>
+      <c r="I171" s="15"/>
+      <c r="J171" s="15"/>
     </row>
     <row r="172" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E172" s="13"/>
-      <c r="F172" s="13"/>
-      <c r="G172" s="13"/>
-      <c r="H172" s="13"/>
-      <c r="I172" s="13"/>
-      <c r="J172" s="13"/>
+      <c r="E172" s="15"/>
+      <c r="F172" s="15"/>
+      <c r="G172" s="15"/>
+      <c r="H172" s="15"/>
+      <c r="I172" s="15"/>
+      <c r="J172" s="15"/>
     </row>
     <row r="173" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E173" s="13"/>
-      <c r="F173" s="13"/>
-      <c r="G173" s="13"/>
-      <c r="H173" s="13"/>
-      <c r="I173" s="13"/>
-      <c r="J173" s="13"/>
+      <c r="E173" s="15"/>
+      <c r="F173" s="15"/>
+      <c r="G173" s="15"/>
+      <c r="H173" s="15"/>
+      <c r="I173" s="15"/>
+      <c r="J173" s="15"/>
     </row>
     <row r="174" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E174" s="13"/>
-      <c r="F174" s="13"/>
-      <c r="G174" s="13"/>
-      <c r="H174" s="13"/>
-      <c r="I174" s="13"/>
-      <c r="J174" s="13"/>
+      <c r="E174" s="15"/>
+      <c r="F174" s="15"/>
+      <c r="G174" s="15"/>
+      <c r="H174" s="15"/>
+      <c r="I174" s="15"/>
+      <c r="J174" s="15"/>
     </row>
     <row r="175" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E175" s="13"/>
-      <c r="F175" s="13"/>
-      <c r="G175" s="13"/>
-      <c r="H175" s="13"/>
-      <c r="I175" s="13"/>
-      <c r="J175" s="13"/>
+      <c r="E175" s="15"/>
+      <c r="F175" s="15"/>
+      <c r="G175" s="15"/>
+      <c r="H175" s="15"/>
+      <c r="I175" s="15"/>
+      <c r="J175" s="15"/>
     </row>
     <row r="176" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E176" s="13"/>
-      <c r="F176" s="13"/>
-      <c r="G176" s="13"/>
-      <c r="H176" s="13"/>
-      <c r="I176" s="13"/>
-      <c r="J176" s="13"/>
+      <c r="E176" s="15"/>
+      <c r="F176" s="15"/>
+      <c r="G176" s="15"/>
+      <c r="H176" s="15"/>
+      <c r="I176" s="15"/>
+      <c r="J176" s="15"/>
     </row>
     <row r="177" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E177" s="13"/>
-      <c r="F177" s="13"/>
-      <c r="G177" s="13"/>
-      <c r="H177" s="13"/>
-      <c r="I177" s="13"/>
-      <c r="J177" s="13"/>
+      <c r="E177" s="15"/>
+      <c r="F177" s="15"/>
+      <c r="G177" s="15"/>
+      <c r="H177" s="15"/>
+      <c r="I177" s="15"/>
+      <c r="J177" s="15"/>
     </row>
     <row r="178" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E178" s="13"/>
-      <c r="F178" s="13"/>
-      <c r="G178" s="13"/>
-      <c r="H178" s="13"/>
-      <c r="I178" s="13"/>
-      <c r="J178" s="13"/>
+      <c r="E178" s="15"/>
+      <c r="F178" s="15"/>
+      <c r="G178" s="15"/>
+      <c r="H178" s="15"/>
+      <c r="I178" s="15"/>
+      <c r="J178" s="15"/>
     </row>
     <row r="179" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E179" s="13"/>
-      <c r="F179" s="13"/>
-      <c r="G179" s="13"/>
-      <c r="H179" s="13"/>
-      <c r="I179" s="13"/>
-      <c r="J179" s="13"/>
+      <c r="E179" s="15"/>
+      <c r="F179" s="15"/>
+      <c r="G179" s="15"/>
+      <c r="H179" s="15"/>
+      <c r="I179" s="15"/>
+      <c r="J179" s="15"/>
     </row>
     <row r="180" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E180" s="13"/>
-      <c r="F180" s="13"/>
-      <c r="G180" s="13"/>
-      <c r="H180" s="13"/>
-      <c r="I180" s="13"/>
-      <c r="J180" s="13"/>
+      <c r="E180" s="15"/>
+      <c r="F180" s="15"/>
+      <c r="G180" s="15"/>
+      <c r="H180" s="15"/>
+      <c r="I180" s="15"/>
+      <c r="J180" s="15"/>
     </row>
     <row r="181" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E181" s="13"/>
-      <c r="F181" s="13"/>
-      <c r="G181" s="13"/>
-      <c r="H181" s="13"/>
-      <c r="I181" s="13"/>
-      <c r="J181" s="13"/>
+      <c r="E181" s="15"/>
+      <c r="F181" s="15"/>
+      <c r="G181" s="15"/>
+      <c r="H181" s="15"/>
+      <c r="I181" s="15"/>
+      <c r="J181" s="15"/>
     </row>
     <row r="182" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E182" s="13"/>
-      <c r="F182" s="13"/>
-      <c r="G182" s="13"/>
-      <c r="H182" s="13"/>
-      <c r="I182" s="13"/>
-      <c r="J182" s="13"/>
+      <c r="E182" s="15"/>
+      <c r="F182" s="15"/>
+      <c r="G182" s="15"/>
+      <c r="H182" s="15"/>
+      <c r="I182" s="15"/>
+      <c r="J182" s="15"/>
     </row>
     <row r="183" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E183" s="13"/>
-      <c r="F183" s="13"/>
-      <c r="G183" s="13"/>
-      <c r="H183" s="13"/>
-      <c r="I183" s="13"/>
-      <c r="J183" s="13"/>
+      <c r="E183" s="15"/>
+      <c r="F183" s="15"/>
+      <c r="G183" s="15"/>
+      <c r="H183" s="15"/>
+      <c r="I183" s="15"/>
+      <c r="J183" s="15"/>
     </row>
     <row r="184" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E184" s="13"/>
-      <c r="F184" s="13"/>
-      <c r="G184" s="13"/>
-      <c r="H184" s="13"/>
-      <c r="I184" s="13"/>
-      <c r="J184" s="13"/>
+      <c r="E184" s="15"/>
+      <c r="F184" s="15"/>
+      <c r="G184" s="15"/>
+      <c r="H184" s="15"/>
+      <c r="I184" s="15"/>
+      <c r="J184" s="15"/>
     </row>
     <row r="185" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E185" s="13"/>
-      <c r="F185" s="13"/>
-      <c r="G185" s="13"/>
-      <c r="H185" s="13"/>
-      <c r="I185" s="13"/>
-      <c r="J185" s="13"/>
+      <c r="E185" s="15"/>
+      <c r="F185" s="15"/>
+      <c r="G185" s="15"/>
+      <c r="H185" s="15"/>
+      <c r="I185" s="15"/>
+      <c r="J185" s="15"/>
     </row>
     <row r="186" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E186" s="13"/>
-      <c r="F186" s="13"/>
-      <c r="G186" s="13"/>
-      <c r="H186" s="13"/>
-      <c r="I186" s="13"/>
-      <c r="J186" s="13"/>
+      <c r="E186" s="15"/>
+      <c r="F186" s="15"/>
+      <c r="G186" s="15"/>
+      <c r="H186" s="15"/>
+      <c r="I186" s="15"/>
+      <c r="J186" s="15"/>
     </row>
     <row r="187" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E187" s="13"/>
-      <c r="F187" s="13"/>
-      <c r="G187" s="13"/>
-      <c r="H187" s="13"/>
-      <c r="I187" s="13"/>
-      <c r="J187" s="13"/>
+      <c r="E187" s="15"/>
+      <c r="F187" s="15"/>
+      <c r="G187" s="15"/>
+      <c r="H187" s="15"/>
+      <c r="I187" s="15"/>
+      <c r="J187" s="15"/>
     </row>
     <row r="188" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E188" s="13"/>
-      <c r="F188" s="13"/>
-      <c r="G188" s="13"/>
-      <c r="H188" s="13"/>
-      <c r="I188" s="13"/>
-      <c r="J188" s="13"/>
+      <c r="E188" s="15"/>
+      <c r="F188" s="15"/>
+      <c r="G188" s="15"/>
+      <c r="H188" s="15"/>
+      <c r="I188" s="15"/>
+      <c r="J188" s="15"/>
     </row>
     <row r="189" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E189" s="13"/>
-      <c r="F189" s="13"/>
-      <c r="G189" s="13"/>
-      <c r="H189" s="13"/>
-      <c r="I189" s="13"/>
-      <c r="J189" s="13"/>
+      <c r="E189" s="15"/>
+      <c r="F189" s="15"/>
+      <c r="G189" s="15"/>
+      <c r="H189" s="15"/>
+      <c r="I189" s="15"/>
+      <c r="J189" s="15"/>
     </row>
     <row r="190" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E190" s="13"/>
-      <c r="F190" s="13"/>
-      <c r="G190" s="13"/>
-      <c r="H190" s="13"/>
-      <c r="I190" s="13"/>
-      <c r="J190" s="13"/>
+      <c r="E190" s="15"/>
+      <c r="F190" s="15"/>
+      <c r="G190" s="15"/>
+      <c r="H190" s="15"/>
+      <c r="I190" s="15"/>
+      <c r="J190" s="15"/>
     </row>
     <row r="191" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E191" s="13"/>
-      <c r="F191" s="13"/>
-      <c r="G191" s="13"/>
-      <c r="H191" s="13"/>
-      <c r="I191" s="13"/>
-      <c r="J191" s="13"/>
+      <c r="E191" s="15"/>
+      <c r="F191" s="15"/>
+      <c r="G191" s="15"/>
+      <c r="H191" s="15"/>
+      <c r="I191" s="15"/>
+      <c r="J191" s="15"/>
     </row>
     <row r="192" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E192" s="13"/>
-      <c r="F192" s="13"/>
-      <c r="G192" s="13"/>
-      <c r="H192" s="13"/>
-      <c r="I192" s="13"/>
-      <c r="J192" s="13"/>
+      <c r="E192" s="15"/>
+      <c r="F192" s="15"/>
+      <c r="G192" s="15"/>
+      <c r="H192" s="15"/>
+      <c r="I192" s="15"/>
+      <c r="J192" s="15"/>
     </row>
     <row r="193" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E193" s="13"/>
-      <c r="F193" s="13"/>
-      <c r="G193" s="13"/>
-      <c r="H193" s="13"/>
-      <c r="I193" s="13"/>
-      <c r="J193" s="13"/>
+      <c r="E193" s="15"/>
+      <c r="F193" s="15"/>
+      <c r="G193" s="15"/>
+      <c r="H193" s="15"/>
+      <c r="I193" s="15"/>
+      <c r="J193" s="15"/>
     </row>
     <row r="194" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E194" s="13"/>
-      <c r="F194" s="13"/>
-      <c r="G194" s="13"/>
-      <c r="H194" s="13"/>
-      <c r="I194" s="13"/>
-      <c r="J194" s="13"/>
+      <c r="E194" s="15"/>
+      <c r="F194" s="15"/>
+      <c r="G194" s="15"/>
+      <c r="H194" s="15"/>
+      <c r="I194" s="15"/>
+      <c r="J194" s="15"/>
     </row>
     <row r="195" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E195" s="13"/>
-      <c r="F195" s="13"/>
-      <c r="G195" s="13"/>
-      <c r="H195" s="13"/>
-      <c r="I195" s="13"/>
-      <c r="J195" s="13"/>
+      <c r="E195" s="15"/>
+      <c r="F195" s="15"/>
+      <c r="G195" s="15"/>
+      <c r="H195" s="15"/>
+      <c r="I195" s="15"/>
+      <c r="J195" s="15"/>
     </row>
     <row r="196" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E196" s="13"/>
-      <c r="F196" s="13"/>
-      <c r="G196" s="13"/>
-      <c r="H196" s="13"/>
-      <c r="I196" s="13"/>
-      <c r="J196" s="13"/>
+      <c r="E196" s="15"/>
+      <c r="F196" s="15"/>
+      <c r="G196" s="15"/>
+      <c r="H196" s="15"/>
+      <c r="I196" s="15"/>
+      <c r="J196" s="15"/>
     </row>
     <row r="197" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E197" s="13"/>
-      <c r="F197" s="13"/>
-      <c r="G197" s="13"/>
-      <c r="H197" s="13"/>
-      <c r="I197" s="13"/>
-      <c r="J197" s="13"/>
+      <c r="E197" s="15"/>
+      <c r="F197" s="15"/>
+      <c r="G197" s="15"/>
+      <c r="H197" s="15"/>
+      <c r="I197" s="15"/>
+      <c r="J197" s="15"/>
     </row>
     <row r="198" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E198" s="13"/>
-      <c r="F198" s="13"/>
-      <c r="G198" s="13"/>
-      <c r="H198" s="13"/>
-      <c r="I198" s="13"/>
-      <c r="J198" s="13"/>
+      <c r="E198" s="15"/>
+      <c r="F198" s="15"/>
+      <c r="G198" s="15"/>
+      <c r="H198" s="15"/>
+      <c r="I198" s="15"/>
+      <c r="J198" s="15"/>
     </row>
     <row r="199" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E199" s="13"/>
-      <c r="F199" s="13"/>
-      <c r="G199" s="13"/>
-      <c r="H199" s="13"/>
-      <c r="I199" s="13"/>
-      <c r="J199" s="13"/>
+      <c r="E199" s="15"/>
+      <c r="F199" s="15"/>
+      <c r="G199" s="15"/>
+      <c r="H199" s="15"/>
+      <c r="I199" s="15"/>
+      <c r="J199" s="15"/>
     </row>
     <row r="200" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E200" s="13"/>
-      <c r="F200" s="13"/>
-      <c r="G200" s="13"/>
-      <c r="H200" s="13"/>
-      <c r="I200" s="13"/>
-      <c r="J200" s="13"/>
+      <c r="E200" s="15"/>
+      <c r="F200" s="15"/>
+      <c r="G200" s="15"/>
+      <c r="H200" s="15"/>
+      <c r="I200" s="15"/>
+      <c r="J200" s="15"/>
     </row>
     <row r="201" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E201" s="13"/>
-      <c r="F201" s="13"/>
-      <c r="G201" s="13"/>
-      <c r="H201" s="13"/>
-      <c r="I201" s="13"/>
-      <c r="J201" s="13"/>
+      <c r="E201" s="15"/>
+      <c r="F201" s="15"/>
+      <c r="G201" s="15"/>
+      <c r="H201" s="15"/>
+      <c r="I201" s="15"/>
+      <c r="J201" s="15"/>
     </row>
     <row r="202" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E202" s="13"/>
-      <c r="F202" s="13"/>
-      <c r="G202" s="13"/>
-      <c r="H202" s="13"/>
-      <c r="I202" s="13"/>
-      <c r="J202" s="13"/>
+      <c r="E202" s="15"/>
+      <c r="F202" s="15"/>
+      <c r="G202" s="15"/>
+      <c r="H202" s="15"/>
+      <c r="I202" s="15"/>
+      <c r="J202" s="15"/>
     </row>
     <row r="203" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E203" s="13"/>
-      <c r="F203" s="13"/>
-      <c r="G203" s="13"/>
-      <c r="H203" s="13"/>
-      <c r="I203" s="13"/>
-      <c r="J203" s="13"/>
+      <c r="E203" s="15"/>
+      <c r="F203" s="15"/>
+      <c r="G203" s="15"/>
+      <c r="H203" s="15"/>
+      <c r="I203" s="15"/>
+      <c r="J203" s="15"/>
     </row>
     <row r="204" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E204" s="13"/>
-      <c r="F204" s="13"/>
-      <c r="G204" s="13"/>
-      <c r="H204" s="13"/>
-      <c r="I204" s="13"/>
-      <c r="J204" s="13"/>
+      <c r="E204" s="15"/>
+      <c r="F204" s="15"/>
+      <c r="G204" s="15"/>
+      <c r="H204" s="15"/>
+      <c r="I204" s="15"/>
+      <c r="J204" s="15"/>
     </row>
     <row r="205" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E205" s="13"/>
-      <c r="F205" s="13"/>
-      <c r="G205" s="13"/>
-      <c r="H205" s="13"/>
-      <c r="I205" s="13"/>
-      <c r="J205" s="13"/>
+      <c r="E205" s="15"/>
+      <c r="F205" s="15"/>
+      <c r="G205" s="15"/>
+      <c r="H205" s="15"/>
+      <c r="I205" s="15"/>
+      <c r="J205" s="15"/>
     </row>
     <row r="206" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E206" s="13"/>
-      <c r="F206" s="13"/>
-      <c r="G206" s="13"/>
-      <c r="H206" s="13"/>
-      <c r="I206" s="13"/>
-      <c r="J206" s="13"/>
+      <c r="E206" s="15"/>
+      <c r="F206" s="15"/>
+      <c r="G206" s="15"/>
+      <c r="H206" s="15"/>
+      <c r="I206" s="15"/>
+      <c r="J206" s="15"/>
     </row>
     <row r="207" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E207" s="13"/>
-      <c r="F207" s="13"/>
-      <c r="G207" s="13"/>
-      <c r="H207" s="13"/>
-      <c r="I207" s="13"/>
-      <c r="J207" s="13"/>
+      <c r="E207" s="15"/>
+      <c r="F207" s="15"/>
+      <c r="G207" s="15"/>
+      <c r="H207" s="15"/>
+      <c r="I207" s="15"/>
+      <c r="J207" s="15"/>
     </row>
     <row r="208" spans="5:10" x14ac:dyDescent="0.2">
-      <c r="E208" s="13"/>
-      <c r="F208" s="13"/>
-      <c r="G208" s="13"/>
-      <c r="H208" s="13"/>
-      <c r="I208" s="13"/>
-      <c r="J208" s="13"/>
+      <c r="E208" s="15"/>
+      <c r="F208" s="15"/>
+      <c r="G208" s="15"/>
+      <c r="H208" s="15"/>
+      <c r="I208" s="15"/>
+      <c r="J208" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2992,7 +2992,7 @@
   <dimension ref="A1:S57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3034,7 +3034,7 @@
       </c>
       <c r="P4" s="11"/>
       <c r="Q4" s="7"/>
-      <c r="S4" s="15"/>
+      <c r="S4" s="13"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
@@ -3045,7 +3045,7 @@
       </c>
       <c r="P5" s="11"/>
       <c r="Q5" s="8"/>
-      <c r="S5" s="14"/>
+      <c r="S5" s="12"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
@@ -3056,7 +3056,7 @@
       </c>
       <c r="P6" s="11"/>
       <c r="Q6" s="8"/>
-      <c r="S6" s="15"/>
+      <c r="S6" s="13"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
@@ -3067,7 +3067,7 @@
       </c>
       <c r="P7" s="11"/>
       <c r="Q7" s="8"/>
-      <c r="S7" s="15"/>
+      <c r="S7" s="13"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
@@ -3078,7 +3078,7 @@
       </c>
       <c r="P8" s="11"/>
       <c r="Q8" s="8"/>
-      <c r="S8" s="14"/>
+      <c r="S8" s="12"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
@@ -3089,7 +3089,7 @@
       </c>
       <c r="P9" s="11"/>
       <c r="Q9" s="8"/>
-      <c r="S9" s="15"/>
+      <c r="S9" s="13"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
@@ -3100,7 +3100,7 @@
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="8"/>
-      <c r="S10" s="15"/>
+      <c r="S10" s="13"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
@@ -3112,7 +3112,7 @@
       <c r="I11" s="9"/>
       <c r="P11" s="11"/>
       <c r="Q11" s="7"/>
-      <c r="S11" s="14"/>
+      <c r="S11" s="12"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
@@ -3124,7 +3124,7 @@
       <c r="I12" s="9"/>
       <c r="P12" s="11"/>
       <c r="Q12" s="8"/>
-      <c r="S12" s="15"/>
+      <c r="S12" s="13"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
@@ -3136,7 +3136,7 @@
       <c r="I13" s="9"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="8"/>
-      <c r="S13" s="15"/>
+      <c r="S13" s="13"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
@@ -3148,7 +3148,7 @@
       <c r="I14" s="9"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="8"/>
-      <c r="S14" s="14"/>
+      <c r="S14" s="12"/>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
@@ -3160,7 +3160,7 @@
       <c r="I15" s="9"/>
       <c r="P15" s="11"/>
       <c r="Q15" s="7"/>
-      <c r="S15" s="15"/>
+      <c r="S15" s="13"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
@@ -3172,7 +3172,7 @@
       <c r="I16" s="9"/>
       <c r="P16" s="11"/>
       <c r="Q16" s="8"/>
-      <c r="S16" s="15"/>
+      <c r="S16" s="13"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
@@ -3184,7 +3184,7 @@
       <c r="I17" s="9"/>
       <c r="P17" s="11"/>
       <c r="Q17" s="8"/>
-      <c r="S17" s="14"/>
+      <c r="S17" s="12"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
@@ -3196,7 +3196,7 @@
       <c r="I18" s="9"/>
       <c r="P18" s="11"/>
       <c r="Q18" s="7"/>
-      <c r="S18" s="15"/>
+      <c r="S18" s="13"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
@@ -3208,7 +3208,7 @@
       <c r="I19" s="9"/>
       <c r="P19" s="11"/>
       <c r="Q19" s="8"/>
-      <c r="S19" s="15"/>
+      <c r="S19" s="13"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
@@ -3220,7 +3220,7 @@
       <c r="I20" s="9"/>
       <c r="P20" s="11"/>
       <c r="Q20" s="8"/>
-      <c r="S20" s="14"/>
+      <c r="S20" s="12"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
@@ -3232,7 +3232,7 @@
       <c r="I21" s="9"/>
       <c r="P21" s="11"/>
       <c r="Q21" s="8"/>
-      <c r="S21" s="15"/>
+      <c r="S21" s="13"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
@@ -3244,7 +3244,7 @@
       <c r="I22" s="9"/>
       <c r="P22" s="11"/>
       <c r="Q22" s="8"/>
-      <c r="S22" s="15"/>
+      <c r="S22" s="13"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
@@ -3256,7 +3256,7 @@
       <c r="I23" s="9"/>
       <c r="P23" s="11"/>
       <c r="Q23" s="8"/>
-      <c r="S23" s="14"/>
+      <c r="S23" s="12"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
@@ -3268,7 +3268,7 @@
       <c r="I24" s="9"/>
       <c r="P24" s="11"/>
       <c r="Q24" s="7"/>
-      <c r="S24" s="15"/>
+      <c r="S24" s="13"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
@@ -3280,7 +3280,7 @@
       <c r="I25" s="9"/>
       <c r="P25" s="11"/>
       <c r="Q25" s="8"/>
-      <c r="S25" s="15"/>
+      <c r="S25" s="13"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
@@ -3292,7 +3292,7 @@
       <c r="I26" s="9"/>
       <c r="P26" s="11"/>
       <c r="Q26" s="8"/>
-      <c r="S26" s="14"/>
+      <c r="S26" s="12"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
@@ -3304,7 +3304,7 @@
       <c r="I27" s="9"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="8"/>
-      <c r="S27" s="15"/>
+      <c r="S27" s="13"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
@@ -3316,7 +3316,7 @@
       <c r="I28" s="9"/>
       <c r="P28" s="11"/>
       <c r="Q28" s="7"/>
-      <c r="S28" s="15"/>
+      <c r="S28" s="13"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
@@ -3328,7 +3328,7 @@
       <c r="I29" s="9"/>
       <c r="P29" s="11"/>
       <c r="Q29" s="8"/>
-      <c r="S29" s="14"/>
+      <c r="S29" s="12"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
@@ -3340,7 +3340,7 @@
       <c r="I30" s="9"/>
       <c r="P30" s="11"/>
       <c r="Q30" s="8"/>
-      <c r="S30" s="15"/>
+      <c r="S30" s="13"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
@@ -3352,7 +3352,7 @@
       <c r="I31" s="9"/>
       <c r="P31" s="11"/>
       <c r="Q31" s="8"/>
-      <c r="S31" s="15"/>
+      <c r="S31" s="13"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
@@ -3364,7 +3364,7 @@
       <c r="I32" s="9"/>
       <c r="P32" s="11"/>
       <c r="Q32" s="7"/>
-      <c r="S32" s="14"/>
+      <c r="S32" s="12"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
@@ -3376,7 +3376,7 @@
       <c r="I33" s="9"/>
       <c r="P33" s="11"/>
       <c r="Q33" s="8"/>
-      <c r="S33" s="15"/>
+      <c r="S33" s="13"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
@@ -3388,7 +3388,7 @@
       <c r="I34" s="9"/>
       <c r="P34" s="11"/>
       <c r="Q34" s="8"/>
-      <c r="S34" s="15"/>
+      <c r="S34" s="13"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
@@ -3400,7 +3400,7 @@
       <c r="I35" s="9"/>
       <c r="P35" s="11"/>
       <c r="Q35" s="8"/>
-      <c r="S35" s="14"/>
+      <c r="S35" s="12"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
@@ -3412,7 +3412,7 @@
       <c r="I36" s="9"/>
       <c r="P36" s="11"/>
       <c r="Q36" s="8"/>
-      <c r="S36" s="15"/>
+      <c r="S36" s="13"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
@@ -3424,7 +3424,7 @@
       <c r="I37" s="9"/>
       <c r="P37" s="11"/>
       <c r="Q37" s="8"/>
-      <c r="S37" s="15"/>
+      <c r="S37" s="13"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
@@ -3436,7 +3436,7 @@
       <c r="I38" s="9"/>
       <c r="P38" s="11"/>
       <c r="Q38" s="8"/>
-      <c r="S38" s="14"/>
+      <c r="S38" s="12"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A39" s="9">
@@ -3448,7 +3448,7 @@
       <c r="I39" s="9"/>
       <c r="P39" s="11"/>
       <c r="Q39" s="8"/>
-      <c r="S39" s="15"/>
+      <c r="S39" s="13"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A40" s="9">
@@ -3460,7 +3460,7 @@
       <c r="I40" s="9"/>
       <c r="P40" s="11"/>
       <c r="Q40" s="8"/>
-      <c r="S40" s="15"/>
+      <c r="S40" s="13"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
@@ -3472,7 +3472,7 @@
       <c r="I41" s="9"/>
       <c r="P41" s="11"/>
       <c r="Q41" s="8"/>
-      <c r="S41" s="14"/>
+      <c r="S41" s="12"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="9">
@@ -3484,7 +3484,7 @@
       <c r="I42" s="9"/>
       <c r="P42" s="11"/>
       <c r="Q42" s="8"/>
-      <c r="S42" s="15"/>
+      <c r="S42" s="13"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
@@ -3496,7 +3496,7 @@
       <c r="I43" s="9"/>
       <c r="P43" s="11"/>
       <c r="Q43" s="8"/>
-      <c r="S43" s="15"/>
+      <c r="S43" s="13"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
@@ -3508,7 +3508,7 @@
       <c r="I44" s="9"/>
       <c r="P44" s="11"/>
       <c r="Q44" s="8"/>
-      <c r="S44" s="14"/>
+      <c r="S44" s="12"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A45" s="9">
@@ -3520,7 +3520,7 @@
       <c r="I45" s="9"/>
       <c r="P45" s="11"/>
       <c r="Q45" s="8"/>
-      <c r="S45" s="15"/>
+      <c r="S45" s="13"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A46" s="9">
@@ -3532,7 +3532,7 @@
       <c r="I46" s="9"/>
       <c r="P46" s="11"/>
       <c r="Q46" s="7"/>
-      <c r="S46" s="15"/>
+      <c r="S46" s="13"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
@@ -3544,7 +3544,7 @@
       <c r="I47" s="9"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="8"/>
-      <c r="S47" s="14"/>
+      <c r="S47" s="12"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
@@ -3556,19 +3556,19 @@
       <c r="I48" s="9"/>
       <c r="P48" s="11"/>
       <c r="Q48" s="7"/>
-      <c r="S48" s="15"/>
+      <c r="S48" s="13"/>
     </row>
     <row r="49" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I49" s="9"/>
       <c r="P49" s="11"/>
       <c r="Q49" s="7"/>
-      <c r="S49" s="15"/>
+      <c r="S49" s="13"/>
     </row>
     <row r="50" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I50" s="9"/>
       <c r="P50" s="11"/>
       <c r="Q50" s="7"/>
-      <c r="S50" s="14"/>
+      <c r="S50" s="12"/>
     </row>
     <row r="51" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I51" s="9"/>

</xml_diff>